<commit_message>
ng: update oncho forms
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2024/cross river/sites.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2024/cross river/sites.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO Thinkpad\Documents\InStrat\NTD Oncho\Cross River\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2024\cross river\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E24062E-BC7E-4DD8-BB1B-0C3D84F890DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5988115E-2C06-433B-A857-BA414CEBA166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="12900" xr2:uid="{EF7B2CDC-01F9-41EF-8CF8-2C5AEBC748FA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF7B2CDC-01F9-41EF-8CF8-2C5AEBC748FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t xml:space="preserve">CRS ONCHO HOT SPOT COMMUNITIES </t>
   </si>
@@ -109,6 +121,42 @@
   </si>
   <si>
     <t>CRS_OGO_M_007</t>
+  </si>
+  <si>
+    <t>AKAMKPA</t>
+  </si>
+  <si>
+    <t>BOKI</t>
+  </si>
+  <si>
+    <t>OGOJA</t>
+  </si>
+  <si>
+    <t>YAKURR</t>
+  </si>
+  <si>
+    <t>AKING</t>
+  </si>
+  <si>
+    <t>AKWA IBAMI</t>
+  </si>
+  <si>
+    <t>EKANG</t>
+  </si>
+  <si>
+    <t>EKONG</t>
+  </si>
+  <si>
+    <t>MFAMOSING</t>
+  </si>
+  <si>
+    <t>OKWA 11</t>
+  </si>
+  <si>
+    <t>OKENDE IDP CAMP</t>
+  </si>
+  <si>
+    <t>AGOI IBAMI</t>
   </si>
 </sst>
 </file>
@@ -188,22 +236,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -217,6 +256,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -236,9 +281,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -276,7 +321,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -382,7 +427,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -524,7 +569,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -534,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249AE3EE-87B4-490A-89C7-40EB900DF942}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,190 +592,190 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>5.4389900000000004</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>8.6389200000000006</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>5.3359699999999997</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <v>8.2360699999999998</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <v>5.6680599999999997</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>8.8171300000000006</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>5.2751000000000001</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <v>8.5562000000000005</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <v>5.1013900000000003</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="6">
         <v>8.5023199999999992</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="6">
         <v>6.3841099999999997</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="6">
         <v>9.1817799999999998</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="4" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="6">
         <v>5.7180099999999996</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="6">
         <v>8.1681500000000007</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -743,7 +788,272 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFC68BD-B4D8-457A-8822-3B2E8ABF91F0}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6">
+        <v>5.4389900000000004</v>
+      </c>
+      <c r="E2" s="6">
+        <v>8.6389200000000006</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="6">
+        <v>5.3359699999999997</v>
+      </c>
+      <c r="E3" s="6">
+        <v>8.2360699999999998</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5.6680599999999997</v>
+      </c>
+      <c r="E4" s="6">
+        <v>8.8171300000000006</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5.2751000000000001</v>
+      </c>
+      <c r="E5" s="6">
+        <v>8.5562000000000005</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5.1013900000000003</v>
+      </c>
+      <c r="E6" s="6">
+        <v>8.5023199999999992</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="6">
+        <v>6.3841099999999997</v>
+      </c>
+      <c r="E7" s="6">
+        <v>9.1817799999999998</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5.7180099999999996</v>
+      </c>
+      <c r="E9" s="6">
+        <v>8.1681500000000007</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:J9">
+    <sortCondition ref="I2:I9"/>
+    <sortCondition ref="J2:J9"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F61D857ACC8084D9287671D8B7E15F4" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0c3a67db788bfb057b2db4972c06362d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92042fd9-f4c9-49ed-97f1-ba485e322b1e" xmlns:ns3="744cc826-a471-4feb-879c-6424ce8a761f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="13059b5e6b4741244ec9ec4e04bff113" ns2:_="" ns3:_="">
     <xsd:import namespace="92042fd9-f4c9-49ed-97f1-ba485e322b1e"/>
@@ -978,19 +1288,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{044C41F6-708A-4426-95A0-4D900CD088EC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59C5A174-177A-4A02-8BD1-16C762A884BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59C5A174-177A-4A02-8BD1-16C762A884BF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{044C41F6-708A-4426-95A0-4D900CD088EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="92042fd9-f4c9-49ed-97f1-ba485e322b1e"/>
+    <ds:schemaRef ds:uri="744cc826-a471-4feb-879c-6424ce8a761f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>